<commit_message>
Updated the data folder
</commit_message>
<xml_diff>
--- a/data/Downtime Tracker.xlsx
+++ b/data/Downtime Tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kenbright-my.sharepoint.com/personal/rochieng_kenbright_africa/Documents/Attachments/projects/2024/October/Downtime Tracker/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kenbright.sharepoint.com/sites/KAFSShinnyAppsModels/Shared Documents/General/IBS Downtime Tracker/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36040CC-F077-4112-89B5-D3780B15BBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{C36040CC-F077-4112-89B5-D3780B15BBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91AB3A7E-3BEB-4FD2-B419-9D7102596739}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1700" yWindow="4080" windowWidth="16800" windowHeight="6000" xr2:uid="{05B4B252-E3B0-4717-B25C-A132C97EFD57}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{05B4B252-E3B0-4717-B25C-A132C97EFD57}"/>
   </bookViews>
   <sheets>
     <sheet name="Downtime Tracker" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="73">
   <si>
     <t>Date</t>
   </si>
@@ -665,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBBAA39-A663-416C-A897-5B0C6D08F651}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -736,7 +736,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>12</v>
@@ -769,7 +769,7 @@
         <v>11</v>
       </c>
       <c r="H3" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>16</v>
@@ -802,7 +802,7 @@
         <v>11</v>
       </c>
       <c r="H4" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>16</v>
@@ -835,7 +835,7 @@
         <v>11</v>
       </c>
       <c r="H5" s="3">
-        <v>11</v>
+        <v>264</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>21</v>
@@ -868,7 +868,7 @@
         <v>11</v>
       </c>
       <c r="H6" s="3">
-        <v>19</v>
+        <v>456</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>23</v>
@@ -901,7 +901,7 @@
         <v>11</v>
       </c>
       <c r="H7" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>25</v>
@@ -934,7 +934,7 @@
         <v>11</v>
       </c>
       <c r="H8" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>25</v>
@@ -967,7 +967,7 @@
         <v>11</v>
       </c>
       <c r="H9" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>29</v>
@@ -1000,7 +1000,7 @@
         <v>11</v>
       </c>
       <c r="H10" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>25</v>
@@ -1033,7 +1033,7 @@
         <v>11</v>
       </c>
       <c r="H11" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>25</v>
@@ -1066,7 +1066,7 @@
         <v>11</v>
       </c>
       <c r="H12" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>25</v>
@@ -1099,7 +1099,7 @@
         <v>35</v>
       </c>
       <c r="H13" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>36</v>
@@ -1132,7 +1132,7 @@
         <v>54</v>
       </c>
       <c r="H14" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>16</v>
@@ -1165,7 +1165,7 @@
         <v>35</v>
       </c>
       <c r="H15" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>16</v>
@@ -1198,7 +1198,7 @@
         <v>35</v>
       </c>
       <c r="H16" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>16</v>
@@ -1231,7 +1231,7 @@
         <v>35</v>
       </c>
       <c r="H17" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>16</v>
@@ -1264,7 +1264,7 @@
         <v>11</v>
       </c>
       <c r="H18" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>16</v>
@@ -1297,7 +1297,7 @@
         <v>11</v>
       </c>
       <c r="H19" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>16</v>
@@ -1330,7 +1330,7 @@
         <v>11</v>
       </c>
       <c r="H20" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>16</v>
@@ -1363,7 +1363,7 @@
         <v>11</v>
       </c>
       <c r="H21" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>16</v>
@@ -1396,7 +1396,7 @@
         <v>11</v>
       </c>
       <c r="H22" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>16</v>
@@ -1429,7 +1429,7 @@
         <v>11</v>
       </c>
       <c r="H23" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>16</v>
@@ -1462,7 +1462,7 @@
         <v>11</v>
       </c>
       <c r="H24" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>16</v>
@@ -1495,7 +1495,7 @@
         <v>11</v>
       </c>
       <c r="H25" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>16</v>
@@ -1528,7 +1528,7 @@
         <v>11</v>
       </c>
       <c r="H26" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I26" s="3" t="s">
         <v>16</v>
@@ -1561,7 +1561,7 @@
         <v>11</v>
       </c>
       <c r="H27" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>16</v>
@@ -1573,7 +1573,7 @@
     </row>
     <row r="28" spans="1:10" ht="16" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
-        <v>45583</v>
+        <v>45309</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>48</v>
@@ -1594,19 +1594,19 @@
         <v>11</v>
       </c>
       <c r="H28" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="0"/>
-        <v>October</v>
+        <v>January</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
-        <v>45617</v>
+        <v>45312</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>58</v>
@@ -1627,19 +1627,19 @@
         <v>11</v>
       </c>
       <c r="H29" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="0"/>
-        <v>November</v>
+        <v>January</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
-        <v>45627</v>
+        <v>45323</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>58</v>
@@ -1660,19 +1660,19 @@
         <v>11</v>
       </c>
       <c r="H30" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="0"/>
-        <v>December</v>
+        <v>February</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
-        <v>45634</v>
+        <v>45330</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>56</v>
@@ -1693,19 +1693,19 @@
         <v>11</v>
       </c>
       <c r="H31" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="0"/>
-        <v>December</v>
+        <v>February</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.45">
       <c r="A32" s="4">
-        <v>45640</v>
+        <v>45336</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>58</v>
@@ -1726,14 +1726,14 @@
         <v>11</v>
       </c>
       <c r="H32" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="0"/>
-        <v>December</v>
+        <v>February</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="16" x14ac:dyDescent="0.45">
@@ -1759,7 +1759,7 @@
         <v>11</v>
       </c>
       <c r="H33" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>16</v>
@@ -1792,7 +1792,7 @@
         <v>11</v>
       </c>
       <c r="H34" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>16</v>
@@ -1825,7 +1825,7 @@
         <v>11</v>
       </c>
       <c r="H35" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>16</v>
@@ -1858,7 +1858,7 @@
         <v>11</v>
       </c>
       <c r="H36" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I36" s="3" t="s">
         <v>16</v>
@@ -1891,7 +1891,7 @@
         <v>11</v>
       </c>
       <c r="H37" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I37" s="3" t="s">
         <v>16</v>
@@ -1924,7 +1924,7 @@
         <v>11</v>
       </c>
       <c r="H38" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>16</v>
@@ -1957,7 +1957,7 @@
         <v>11</v>
       </c>
       <c r="H39" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I39" s="3" t="s">
         <v>16</v>
@@ -1990,7 +1990,7 @@
         <v>11</v>
       </c>
       <c r="H40" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I40" s="3" t="s">
         <v>16</v>
@@ -2023,7 +2023,7 @@
         <v>11</v>
       </c>
       <c r="H41" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I41" s="3" t="s">
         <v>16</v>
@@ -2056,7 +2056,7 @@
         <v>11</v>
       </c>
       <c r="H42" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>16</v>
@@ -2089,7 +2089,7 @@
         <v>11</v>
       </c>
       <c r="H43" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="I43" s="3" t="s">
         <v>16</v>
@@ -2122,7 +2122,7 @@
         <v>11</v>
       </c>
       <c r="H44" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>16</v>
@@ -2155,7 +2155,7 @@
         <v>11</v>
       </c>
       <c r="H45" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="I45" s="3" t="s">
         <v>16</v>
@@ -2187,7 +2187,9 @@
       <c r="G46" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H46" s="5"/>
+      <c r="H46" s="5">
+        <v>24</v>
+      </c>
       <c r="I46" s="3" t="s">
         <v>16</v>
       </c>
@@ -2219,7 +2221,7 @@
         <v>11</v>
       </c>
       <c r="H47" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>16</v>
@@ -2252,7 +2254,7 @@
         <v>11</v>
       </c>
       <c r="H48" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I48" s="3" t="s">
         <v>16</v>
@@ -2281,9 +2283,15 @@
       <c r="F49" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
+      <c r="G49" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" s="5">
+        <v>12</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="J49" t="str">
         <f t="shared" si="0"/>
         <v>October</v>
@@ -2519,15 +2527,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eaf0034b-6475-43ff-84f3-1a043af659f0" xsi:nil="true"/>
@@ -2538,14 +2537,49 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D2FB91D-0AAB-400F-A371-D8A60590518F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D2FB91D-0AAB-400F-A371-D8A60590518F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2fde81b7-13e2-40b8-9c3f-3c2e0d0d2bcd"/>
+    <ds:schemaRef ds:uri="eaf0034b-6475-43ff-84f3-1a043af659f0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60DEBE6-6A36-4D81-8952-EB0DC2D850DA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53208C9-FE26-43CC-BF3E-D9D7F113A27A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="eaf0034b-6475-43ff-84f3-1a043af659f0"/>
+    <ds:schemaRef ds:uri="2fde81b7-13e2-40b8-9c3f-3c2e0d0d2bcd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53208C9-FE26-43CC-BF3E-D9D7F113A27A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60DEBE6-6A36-4D81-8952-EB0DC2D850DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated the column names
</commit_message>
<xml_diff>
--- a/data/Downtime Tracker.xlsx
+++ b/data/Downtime Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kenbright.sharepoint.com/sites/KAFSShinnyAppsModels/Shared Documents/General/IBS Downtime Tracker/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{C36040CC-F077-4112-89B5-D3780B15BBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91AB3A7E-3BEB-4FD2-B419-9D7102596739}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{C36040CC-F077-4112-89B5-D3780B15BBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7EECFC8-EA13-4105-B540-FF88C31ABA15}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{05B4B252-E3B0-4717-B25C-A132C97EFD57}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{05B4B252-E3B0-4717-B25C-A132C97EFD57}"/>
   </bookViews>
   <sheets>
     <sheet name="Downtime Tracker" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="69">
   <si>
     <t>Date</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Effect</t>
   </si>
   <si>
-    <t>Discovered by</t>
-  </si>
-  <si>
     <t>Reported to</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>Permanent Resolution</t>
   </si>
   <si>
-    <t>Vic - Random Platform test</t>
-  </si>
-  <si>
     <t>Mark - Physical Demo/Illustration</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
     <t>All systems down</t>
   </si>
   <si>
-    <t>Joan, night shift</t>
-  </si>
-  <si>
     <t>Mark - Phone, then Kaki</t>
   </si>
   <si>
@@ -140,9 +131,6 @@
     <t>Mark - Shared Screenshots</t>
   </si>
   <si>
-    <t>Ezekiel - through client</t>
-  </si>
-  <si>
     <t>Mark - Shared Screenshot</t>
   </si>
   <si>
@@ -152,15 +140,9 @@
     <t>Undetermined</t>
   </si>
   <si>
-    <t>Night Shift, Ezekiel</t>
-  </si>
-  <si>
     <t>Mark - Shared screenshots</t>
   </si>
   <si>
-    <t>Vic - Random Test</t>
-  </si>
-  <si>
     <t>Unconcluded</t>
   </si>
   <si>
@@ -173,12 +155,6 @@
     <t>Mark - via Chat</t>
   </si>
   <si>
-    <t>Ezekiel - Random Test</t>
-  </si>
-  <si>
-    <t>Patricia - Call Center Alert</t>
-  </si>
-  <si>
     <t>Mark</t>
   </si>
   <si>
@@ -188,18 +164,6 @@
     <t>Vehicle.co.ke Down</t>
   </si>
   <si>
-    <t>Vic - Call Center Alert</t>
-  </si>
-  <si>
-    <t>Gilbert - Random Test</t>
-  </si>
-  <si>
-    <t>Vic - Observation</t>
-  </si>
-  <si>
-    <t>Vic &amp; Patricia</t>
-  </si>
-  <si>
     <t>Stella</t>
   </si>
   <si>
@@ -258,6 +222,30 @@
   </si>
   <si>
     <t>Month</t>
+  </si>
+  <si>
+    <t>Victor</t>
+  </si>
+  <si>
+    <t>Joan</t>
+  </si>
+  <si>
+    <t>Ezekiel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ezekiel </t>
+  </si>
+  <si>
+    <t>Patricia</t>
+  </si>
+  <si>
+    <t>Gilbert</t>
+  </si>
+  <si>
+    <t>Victor &amp; Patricia</t>
+  </si>
+  <si>
+    <t>Discovered_by</t>
   </si>
 </sst>
 </file>
@@ -665,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBBAA39-A663-416C-A897-5B0C6D08F651}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -692,25 +680,25 @@
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" s="7" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.45">
@@ -718,28 +706,28 @@
         <v>44909</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H2" s="3">
         <v>48</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J2" t="str">
         <f>TEXT(A2, "mmmm")</f>
@@ -751,28 +739,28 @@
         <v>44909</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H3" s="3">
         <v>12</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" ref="J3:J49" si="0">TEXT(A3, "mmmm")</f>
@@ -784,28 +772,28 @@
         <v>44943</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H4" s="3">
         <v>12</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
@@ -817,28 +805,28 @@
         <v>45049</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H5" s="3">
         <v>264</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
@@ -850,28 +838,28 @@
         <v>45054</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H6" s="3">
         <v>456</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
@@ -883,28 +871,28 @@
         <v>45083</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H7" s="3">
         <v>48</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
@@ -916,28 +904,28 @@
         <v>45083</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H8" s="3">
         <v>24</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
@@ -949,28 +937,28 @@
         <v>45090</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H9" s="3">
         <v>48</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
@@ -982,28 +970,28 @@
         <v>45090</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H10" s="3">
         <v>12</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
@@ -1015,28 +1003,28 @@
         <v>45091</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H11" s="3">
         <v>24</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
@@ -1048,28 +1036,28 @@
         <v>45091</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H12" s="3">
         <v>24</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="0"/>
@@ -1081,28 +1069,28 @@
         <v>45092</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H13" s="3">
         <v>48</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
@@ -1114,28 +1102,28 @@
         <v>45099</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="H14" s="3">
         <v>24</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="0"/>
@@ -1147,28 +1135,28 @@
         <v>45099</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H15" s="3">
         <v>12</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="0"/>
@@ -1180,28 +1168,28 @@
         <v>45103</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H16" s="3">
         <v>12</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="0"/>
@@ -1213,28 +1201,28 @@
         <v>45105</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H17" s="3">
         <v>48</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="0"/>
@@ -1246,28 +1234,28 @@
         <v>45106</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H18" s="3">
         <v>12</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="0"/>
@@ -1279,28 +1267,28 @@
         <v>45479</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H19" s="3">
         <v>48</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="0"/>
@@ -1312,28 +1300,28 @@
         <v>45522</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H20" s="3">
         <v>24</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="0"/>
@@ -1345,28 +1333,28 @@
         <v>45526</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H21" s="3">
         <v>12</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="0"/>
@@ -1378,28 +1366,28 @@
         <v>45534</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H22" s="3">
         <v>48</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="0"/>
@@ -1411,28 +1399,28 @@
         <v>45534</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H23" s="3">
         <v>48</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="0"/>
@@ -1444,28 +1432,28 @@
         <v>45549</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H24" s="3">
         <v>24</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="0"/>
@@ -1477,28 +1465,28 @@
         <v>45549</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H25" s="3">
         <v>24</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
@@ -1510,28 +1498,28 @@
         <v>45563</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H26" s="3">
         <v>12</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="0"/>
@@ -1543,28 +1531,28 @@
         <v>45563</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H27" s="3">
         <v>12</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="0"/>
@@ -1576,28 +1564,28 @@
         <v>45309</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H28" s="3">
         <v>12</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="0"/>
@@ -1609,28 +1597,28 @@
         <v>45312</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H29" s="3">
         <v>12</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="0"/>
@@ -1642,28 +1630,28 @@
         <v>45323</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H30" s="3">
         <v>12</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="0"/>
@@ -1675,28 +1663,28 @@
         <v>45330</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H31" s="3">
         <v>12</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="0"/>
@@ -1708,28 +1696,28 @@
         <v>45336</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H32" s="3">
         <v>48</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="0"/>
@@ -1741,28 +1729,28 @@
         <v>45354</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="D33" s="3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H33" s="3">
         <v>12</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J33" t="str">
         <f t="shared" si="0"/>
@@ -1774,28 +1762,28 @@
         <v>45356</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="D34" s="3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H34" s="3">
         <v>12</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J34" t="str">
         <f t="shared" si="0"/>
@@ -1807,28 +1795,28 @@
         <v>45357</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="D35" s="3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H35" s="3">
         <v>12</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="0"/>
@@ -1840,28 +1828,28 @@
         <v>45361</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="D36" s="3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H36" s="3">
         <v>12</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J36" t="str">
         <f t="shared" si="0"/>
@@ -1873,28 +1861,28 @@
         <v>45365</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="D37" s="3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H37" s="3">
         <v>12</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J37" t="str">
         <f t="shared" si="0"/>
@@ -1906,28 +1894,28 @@
         <v>45367</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="D38" s="3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H38" s="3">
         <v>12</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J38" t="str">
         <f t="shared" si="0"/>
@@ -1939,28 +1927,28 @@
         <v>45369</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="D39" s="3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H39" s="3">
         <v>12</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J39" t="str">
         <f t="shared" si="0"/>
@@ -1972,28 +1960,28 @@
         <v>45372</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H40" s="3">
         <v>12</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J40" t="str">
         <f t="shared" si="0"/>
@@ -2005,28 +1993,28 @@
         <v>45377</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="D41" s="3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H41" s="3">
         <v>12</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J41" t="str">
         <f t="shared" si="0"/>
@@ -2038,28 +2026,28 @@
         <v>45399</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H42" s="3">
         <v>12</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J42" t="str">
         <f t="shared" si="0"/>
@@ -2071,28 +2059,28 @@
         <v>45404</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H43" s="3">
         <v>48</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J43" t="str">
         <f t="shared" si="0"/>
@@ -2104,28 +2092,28 @@
         <v>45411</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H44" s="3">
         <v>24</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J44" t="str">
         <f t="shared" si="0"/>
@@ -2137,28 +2125,28 @@
         <v>45412</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H45" s="3">
         <v>48</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J45" t="str">
         <f t="shared" si="0"/>
@@ -2170,28 +2158,28 @@
         <v>45416</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H46" s="5">
         <v>24</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J46" t="str">
         <f t="shared" si="0"/>
@@ -2203,28 +2191,28 @@
         <v>45547</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="D47" s="3" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H47" s="3">
         <v>12</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J47" t="str">
         <f t="shared" si="0"/>
@@ -2236,28 +2224,28 @@
         <v>45574</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C48" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="E48" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H48" s="3">
         <v>24</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J48" t="str">
         <f t="shared" si="0"/>
@@ -2269,28 +2257,28 @@
         <v>45593</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H49" s="5">
         <v>12</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J49" t="str">
         <f t="shared" si="0"/>

</xml_diff>